<commit_message>
Version 1.1. Commentes added
</commit_message>
<xml_diff>
--- a/Assignment01/Design_01.xlsx
+++ b/Assignment01/Design_01.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documentos\CANADA\COLLEGE\2_TERM\2_CSD2354_ProgrammingC#NET\Assignments\Assignment_1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documentos\CANADA\COLLEGE\2_TERM\2_CSD2354_ProgrammingC#NET\Github_Repository\Assignments\Assignment01\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73AB0540-58A7-43C3-80AD-D70C4EF75A84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E969D48-C289-4FB5-AA9B-44A5E680135D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{3C4068DF-F92D-4EAA-A5F6-4C8557B6631E}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{3C4068DF-F92D-4EAA-A5F6-4C8557B6631E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -445,9 +445,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -475,6 +472,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -484,10 +487,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -806,8 +806,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B91CE22C-7D43-4C9F-814A-330414B31299}">
   <dimension ref="A1:C108"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="I90" sqref="I90"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="A50" sqref="A50:C50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -817,1030 +817,1060 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
     </row>
     <row r="2" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="6" t="s">
+      <c r="B3" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="5" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="12" t="s">
+      <c r="A4" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" s="8" t="s">
+      <c r="B4" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="7" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="13"/>
+      <c r="A5" s="14"/>
       <c r="B5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C5" s="8" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="14"/>
-      <c r="B6" s="10" t="s">
+      <c r="A6" s="15"/>
+      <c r="B6" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="11">
+      <c r="C6" s="10">
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="12" t="s">
+      <c r="A7" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" s="8" t="s">
+      <c r="B7" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="7" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="13"/>
+      <c r="A8" s="14"/>
       <c r="B8" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="C8" s="8" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="14"/>
-      <c r="B9" s="10" t="s">
+      <c r="A9" s="15"/>
+      <c r="B9" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="11">
+      <c r="C9" s="10">
         <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="12" t="s">
+      <c r="A10" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C10" s="8" t="s">
+      <c r="B10" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="7" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" s="13"/>
+      <c r="A11" s="14"/>
       <c r="B11" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C11" s="9" t="s">
+      <c r="C11" s="8" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="14"/>
-      <c r="B12" s="10" t="s">
+      <c r="A12" s="15"/>
+      <c r="B12" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="11">
+      <c r="C12" s="10">
         <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" s="12" t="s">
+      <c r="A13" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C13" s="8" t="s">
+      <c r="B13" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" s="7" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" s="13"/>
+      <c r="A14" s="14"/>
       <c r="B14" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C14" s="9" t="s">
+      <c r="C14" s="8" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="14"/>
-      <c r="B15" s="10" t="s">
+      <c r="A15" s="15"/>
+      <c r="B15" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C15" s="11">
+      <c r="C15" s="10">
         <v>3</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" s="12" t="s">
+      <c r="A16" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="B16" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C16" s="8" t="s">
+      <c r="B16" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16" s="7" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" s="13"/>
+      <c r="A17" s="14"/>
       <c r="B17" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C17" s="9" t="s">
+      <c r="C17" s="8" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="14"/>
-      <c r="B18" s="10" t="s">
+      <c r="A18" s="15"/>
+      <c r="B18" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C18" s="11">
+      <c r="C18" s="10">
         <v>4</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" s="2" t="s">
+      <c r="A20" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
+      <c r="B20" s="16"/>
+      <c r="C20" s="16"/>
     </row>
     <row r="21" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="3" t="s">
+      <c r="A21" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="B21" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C21" s="3" t="s">
+      <c r="C21" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="4" t="s">
+      <c r="A22" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B22" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C22" s="6" t="s">
+      <c r="B22" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C22" s="5" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A23" s="12" t="s">
+      <c r="A23" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="B23" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="C23" s="8" t="s">
+      <c r="B23" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C23" s="7" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A24" s="13"/>
+      <c r="A24" s="14"/>
       <c r="B24" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C24" s="9" t="s">
+      <c r="C24" s="8" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="14"/>
-      <c r="B25" s="10" t="s">
+      <c r="A25" s="15"/>
+      <c r="B25" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C25" s="11">
+      <c r="C25" s="10">
         <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A26" s="12" t="s">
+      <c r="A26" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="B26" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C26" s="8" t="s">
+      <c r="B26" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C26" s="7" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="14"/>
-      <c r="B27" s="10" t="s">
+      <c r="A27" s="15"/>
+      <c r="B27" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C27" s="11">
+      <c r="C27" s="10">
         <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A28" s="12" t="s">
+      <c r="A28" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="B28" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="C28" s="8" t="s">
+      <c r="B28" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C28" s="7" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="13"/>
+      <c r="A29" s="14"/>
       <c r="B29" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C29" s="9" t="s">
+      <c r="C29" s="8" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A30" s="12" t="s">
+      <c r="A30" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="B30" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C30" s="8" t="s">
+      <c r="B30" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C30" s="7" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A31" s="13"/>
-      <c r="B31" s="15" t="s">
+      <c r="A31" s="14"/>
+      <c r="B31" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="C31" s="16" t="b">
+      <c r="C31" s="12" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="14"/>
-      <c r="B32" s="10" t="s">
+      <c r="A32" s="15"/>
+      <c r="B32" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="C32" s="11" t="b">
+      <c r="C32" s="10" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A33" s="12" t="s">
+      <c r="A33" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="B33" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="C33" s="8" t="s">
+      <c r="B33" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C33" s="7" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="13"/>
+      <c r="A34" s="14"/>
       <c r="B34" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C34" s="9" t="s">
+      <c r="C34" s="8" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A35" s="12" t="s">
+      <c r="A35" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="B35" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C35" s="8" t="s">
+      <c r="B35" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C35" s="7" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A36" s="13"/>
-      <c r="B36" s="15" t="s">
+      <c r="A36" s="14"/>
+      <c r="B36" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="C36" s="16" t="b">
+      <c r="C36" s="12" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="14"/>
-      <c r="B37" s="10" t="s">
+      <c r="A37" s="15"/>
+      <c r="B37" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="C37" s="11" t="b">
+      <c r="C37" s="10" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A38" s="12" t="s">
+      <c r="A38" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="B38" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="C38" s="8" t="s">
+      <c r="B38" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C38" s="7" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="13"/>
+      <c r="A39" s="14"/>
       <c r="B39" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C39" s="9" t="s">
+      <c r="C39" s="8" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A40" s="12" t="s">
+      <c r="A40" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="B40" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C40" s="8" t="s">
+      <c r="B40" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C40" s="7" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A41" s="13"/>
-      <c r="B41" s="15" t="s">
+      <c r="A41" s="14"/>
+      <c r="B41" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="C41" s="16" t="b">
+      <c r="C41" s="12" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="14"/>
-      <c r="B42" s="10" t="s">
+      <c r="A42" s="15"/>
+      <c r="B42" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="C42" s="11" t="b">
+      <c r="C42" s="10" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A43" s="12" t="s">
+      <c r="A43" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="B43" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C43" s="8" t="s">
+      <c r="B43" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C43" s="7" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A44" s="13"/>
+      <c r="A44" s="14"/>
       <c r="B44" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C44" s="9" t="s">
+      <c r="C44" s="8" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="14"/>
-      <c r="B45" s="10" t="s">
+      <c r="A45" s="15"/>
+      <c r="B45" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C45" s="11">
+      <c r="C45" s="10">
         <v>2</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A46" s="12" t="s">
+      <c r="A46" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B46" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C46" s="8" t="s">
+      <c r="B46" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C46" s="7" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A47" s="13"/>
+      <c r="A47" s="14"/>
       <c r="B47" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C47" s="9" t="s">
+      <c r="C47" s="8" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A48" s="14"/>
-      <c r="B48" s="10" t="s">
+      <c r="A48" s="15"/>
+      <c r="B48" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C48" s="11">
+      <c r="C48" s="10">
         <v>3</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A50" s="2" t="s">
+      <c r="A50" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="B50" s="2"/>
-      <c r="C50" s="2"/>
+      <c r="B50" s="16"/>
+      <c r="C50" s="16"/>
     </row>
     <row r="51" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A51" s="3" t="s">
+      <c r="A51" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B51" s="3" t="s">
+      <c r="B51" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C51" s="3" t="s">
+      <c r="C51" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="52" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A52" s="4" t="s">
+      <c r="A52" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B52" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C52" s="6" t="s">
+      <c r="B52" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C52" s="5" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A53" s="12" t="s">
+      <c r="A53" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="B53" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="C53" s="8" t="s">
+      <c r="B53" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C53" s="7" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A54" s="13"/>
+      <c r="A54" s="14"/>
       <c r="B54" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C54" s="9" t="s">
+      <c r="C54" s="8" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="55" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A55" s="14"/>
-      <c r="B55" s="10" t="s">
+      <c r="A55" s="15"/>
+      <c r="B55" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C55" s="11">
+      <c r="C55" s="10">
         <v>0</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A56" s="12" t="s">
+      <c r="A56" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="B56" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C56" s="8" t="s">
+      <c r="B56" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C56" s="7" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="57" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A57" s="14"/>
-      <c r="B57" s="10" t="s">
+      <c r="A57" s="15"/>
+      <c r="B57" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C57" s="11">
+      <c r="C57" s="10">
         <v>1</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A58" s="12" t="s">
+      <c r="A58" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="B58" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="C58" s="8" t="s">
+      <c r="B58" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C58" s="7" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="59" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A59" s="13"/>
+      <c r="A59" s="14"/>
       <c r="B59" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C59" s="9" t="s">
+      <c r="C59" s="8" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A60" s="12" t="s">
+      <c r="A60" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="B60" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C60" s="8" t="s">
+      <c r="B60" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C60" s="7" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A61" s="13"/>
-      <c r="B61" s="15" t="s">
+      <c r="A61" s="14"/>
+      <c r="B61" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="C61" s="16" t="b">
+      <c r="C61" s="12" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="62" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A62" s="14"/>
-      <c r="B62" s="10" t="s">
+      <c r="A62" s="15"/>
+      <c r="B62" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="C62" s="11" t="b">
+      <c r="C62" s="10" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A63" s="12" t="s">
+      <c r="A63" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="B63" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="C63" s="8" t="s">
+      <c r="B63" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C63" s="7" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="64" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A64" s="13"/>
+      <c r="A64" s="14"/>
       <c r="B64" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C64" s="9" t="s">
+      <c r="C64" s="8" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A65" s="12" t="s">
+      <c r="A65" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="B65" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C65" s="8" t="s">
+      <c r="B65" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C65" s="7" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A66" s="13"/>
-      <c r="B66" s="15" t="s">
+      <c r="A66" s="14"/>
+      <c r="B66" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="C66" s="16" t="b">
+      <c r="C66" s="12" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="67" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A67" s="14"/>
-      <c r="B67" s="10" t="s">
+      <c r="A67" s="15"/>
+      <c r="B67" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="C67" s="11" t="b">
+      <c r="C67" s="10" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A68" s="12" t="s">
+      <c r="A68" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="B68" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="C68" s="8" t="s">
+      <c r="B68" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C68" s="7" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="69" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A69" s="13"/>
+      <c r="A69" s="14"/>
       <c r="B69" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C69" s="9" t="s">
+      <c r="C69" s="8" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A70" s="12" t="s">
+      <c r="A70" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="B70" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C70" s="8" t="s">
+      <c r="B70" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C70" s="7" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A71" s="13"/>
-      <c r="B71" s="15" t="s">
+      <c r="A71" s="14"/>
+      <c r="B71" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="C71" s="16" t="b">
+      <c r="C71" s="12" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="72" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A72" s="14"/>
-      <c r="B72" s="10" t="s">
+      <c r="A72" s="15"/>
+      <c r="B72" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="C72" s="11" t="b">
+      <c r="C72" s="10" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A73" s="12" t="s">
+      <c r="A73" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="B73" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C73" s="8" t="s">
+      <c r="B73" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C73" s="7" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A74" s="13"/>
+      <c r="A74" s="14"/>
       <c r="B74" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C74" s="9" t="s">
+      <c r="C74" s="8" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="75" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A75" s="14"/>
-      <c r="B75" s="10" t="s">
+      <c r="A75" s="15"/>
+      <c r="B75" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C75" s="11">
+      <c r="C75" s="10">
         <v>2</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A76" s="12" t="s">
+      <c r="A76" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B76" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C76" s="8" t="s">
+      <c r="B76" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C76" s="7" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A77" s="13"/>
+      <c r="A77" s="14"/>
       <c r="B77" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C77" s="9" t="s">
+      <c r="C77" s="8" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="78" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A78" s="14"/>
-      <c r="B78" s="10" t="s">
+      <c r="A78" s="15"/>
+      <c r="B78" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C78" s="11">
+      <c r="C78" s="10">
         <v>3</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A80" s="2" t="s">
+      <c r="A80" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="B80" s="2"/>
-      <c r="C80" s="2"/>
+      <c r="B80" s="16"/>
+      <c r="C80" s="16"/>
     </row>
     <row r="81" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A81" s="3" t="s">
+      <c r="A81" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B81" s="3" t="s">
+      <c r="B81" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C81" s="3" t="s">
+      <c r="C81" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="82" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A82" s="4" t="s">
+      <c r="A82" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B82" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C82" s="6" t="s">
+      <c r="B82" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C82" s="5" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A83" s="12" t="s">
+      <c r="A83" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="B83" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="C83" s="8" t="s">
+      <c r="B83" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C83" s="7" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A84" s="13"/>
+      <c r="A84" s="14"/>
       <c r="B84" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C84" s="9" t="s">
+      <c r="C84" s="8" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="85" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A85" s="14"/>
-      <c r="B85" s="10" t="s">
+      <c r="A85" s="15"/>
+      <c r="B85" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C85" s="11">
+      <c r="C85" s="10">
         <v>0</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A86" s="12" t="s">
+      <c r="A86" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="B86" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C86" s="8" t="s">
+      <c r="B86" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C86" s="7" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="87" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A87" s="14"/>
-      <c r="B87" s="10" t="s">
+      <c r="A87" s="15"/>
+      <c r="B87" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C87" s="11">
+      <c r="C87" s="10">
         <v>1</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A88" s="12" t="s">
+      <c r="A88" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="B88" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="C88" s="8" t="s">
+      <c r="B88" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C88" s="7" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="89" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A89" s="13"/>
+      <c r="A89" s="14"/>
       <c r="B89" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C89" s="9" t="s">
+      <c r="C89" s="8" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A90" s="12" t="s">
+      <c r="A90" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="B90" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C90" s="8" t="s">
+      <c r="B90" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C90" s="7" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A91" s="13"/>
-      <c r="B91" s="15" t="s">
+      <c r="A91" s="14"/>
+      <c r="B91" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="C91" s="16" t="b">
+      <c r="C91" s="12" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="92" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A92" s="14"/>
-      <c r="B92" s="10" t="s">
+      <c r="A92" s="15"/>
+      <c r="B92" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="C92" s="11" t="b">
+      <c r="C92" s="10" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A93" s="12" t="s">
+      <c r="A93" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="B93" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="C93" s="8" t="s">
+      <c r="B93" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C93" s="7" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="94" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A94" s="13"/>
+      <c r="A94" s="14"/>
       <c r="B94" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C94" s="9" t="s">
+      <c r="C94" s="8" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A95" s="12" t="s">
+      <c r="A95" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="B95" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C95" s="8" t="s">
+      <c r="B95" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C95" s="7" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A96" s="13"/>
-      <c r="B96" s="15" t="s">
+      <c r="A96" s="14"/>
+      <c r="B96" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="C96" s="16" t="b">
+      <c r="C96" s="12" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="97" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A97" s="14"/>
-      <c r="B97" s="10" t="s">
+      <c r="A97" s="15"/>
+      <c r="B97" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="C97" s="11" t="b">
+      <c r="C97" s="10" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A98" s="12" t="s">
+      <c r="A98" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="B98" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="C98" s="8" t="s">
+      <c r="B98" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C98" s="7" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="99" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A99" s="13"/>
+      <c r="A99" s="14"/>
       <c r="B99" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C99" s="9" t="s">
+      <c r="C99" s="8" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A100" s="12" t="s">
+      <c r="A100" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="B100" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C100" s="8" t="s">
+      <c r="B100" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C100" s="7" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A101" s="13"/>
-      <c r="B101" s="15" t="s">
+      <c r="A101" s="14"/>
+      <c r="B101" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="C101" s="16" t="b">
+      <c r="C101" s="12" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="102" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A102" s="14"/>
-      <c r="B102" s="10" t="s">
+      <c r="A102" s="15"/>
+      <c r="B102" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="C102" s="11" t="b">
+      <c r="C102" s="10" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A103" s="12" t="s">
+      <c r="A103" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="B103" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C103" s="8" t="s">
+      <c r="B103" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C103" s="7" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A104" s="13"/>
+      <c r="A104" s="14"/>
       <c r="B104" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C104" s="9" t="s">
+      <c r="C104" s="8" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="105" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A105" s="14"/>
-      <c r="B105" s="10" t="s">
+      <c r="A105" s="15"/>
+      <c r="B105" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C105" s="11">
+      <c r="C105" s="10">
         <v>2</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A106" s="12" t="s">
+      <c r="A106" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B106" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C106" s="8" t="s">
+      <c r="B106" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C106" s="7" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A107" s="13"/>
+      <c r="A107" s="14"/>
       <c r="B107" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C107" s="9" t="s">
+      <c r="C107" s="8" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="108" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A108" s="14"/>
-      <c r="B108" s="10" t="s">
+      <c r="A108" s="15"/>
+      <c r="B108" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C108" s="11">
+      <c r="C108" s="10">
         <v>3</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="39">
+    <mergeCell ref="A16:A18"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A4:A6"/>
+    <mergeCell ref="A7:A9"/>
+    <mergeCell ref="A10:A12"/>
+    <mergeCell ref="A13:A15"/>
+    <mergeCell ref="A50:C50"/>
+    <mergeCell ref="A20:C20"/>
+    <mergeCell ref="A23:A25"/>
+    <mergeCell ref="A26:A27"/>
+    <mergeCell ref="A28:A29"/>
+    <mergeCell ref="A30:A32"/>
+    <mergeCell ref="A33:A34"/>
+    <mergeCell ref="A35:A37"/>
+    <mergeCell ref="A40:A42"/>
+    <mergeCell ref="A43:A45"/>
+    <mergeCell ref="A38:A39"/>
+    <mergeCell ref="A46:A48"/>
+    <mergeCell ref="A83:A85"/>
+    <mergeCell ref="A53:A55"/>
+    <mergeCell ref="A56:A57"/>
+    <mergeCell ref="A58:A59"/>
+    <mergeCell ref="A60:A62"/>
+    <mergeCell ref="A63:A64"/>
+    <mergeCell ref="A65:A67"/>
+    <mergeCell ref="A68:A69"/>
+    <mergeCell ref="A70:A72"/>
+    <mergeCell ref="A73:A75"/>
+    <mergeCell ref="A76:A78"/>
+    <mergeCell ref="A80:C80"/>
     <mergeCell ref="A100:A102"/>
     <mergeCell ref="A103:A105"/>
     <mergeCell ref="A106:A108"/>
@@ -1850,36 +1880,6 @@
     <mergeCell ref="A93:A94"/>
     <mergeCell ref="A95:A97"/>
     <mergeCell ref="A98:A99"/>
-    <mergeCell ref="A68:A69"/>
-    <mergeCell ref="A70:A72"/>
-    <mergeCell ref="A73:A75"/>
-    <mergeCell ref="A76:A78"/>
-    <mergeCell ref="A80:C80"/>
-    <mergeCell ref="A83:A85"/>
-    <mergeCell ref="A53:A55"/>
-    <mergeCell ref="A56:A57"/>
-    <mergeCell ref="A58:A59"/>
-    <mergeCell ref="A60:A62"/>
-    <mergeCell ref="A63:A64"/>
-    <mergeCell ref="A65:A67"/>
-    <mergeCell ref="A35:A37"/>
-    <mergeCell ref="A40:A42"/>
-    <mergeCell ref="A43:A45"/>
-    <mergeCell ref="A38:A39"/>
-    <mergeCell ref="A46:A48"/>
-    <mergeCell ref="A50:C50"/>
-    <mergeCell ref="A20:C20"/>
-    <mergeCell ref="A23:A25"/>
-    <mergeCell ref="A26:A27"/>
-    <mergeCell ref="A28:A29"/>
-    <mergeCell ref="A30:A32"/>
-    <mergeCell ref="A33:A34"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A4:A6"/>
-    <mergeCell ref="A7:A9"/>
-    <mergeCell ref="A10:A12"/>
-    <mergeCell ref="A13:A15"/>
-    <mergeCell ref="A16:A18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>